<commit_message>
Last revision of epi map
</commit_message>
<xml_diff>
--- a/tigapublic/templates/epi/epi_template.xlsx
+++ b/tigapublic/templates/epi/epi_template.xlsx
@@ -16,40 +16,40 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
   <si>
-    <t>codi</t>
-  </si>
-  <si>
-    <t>centre</t>
-  </si>
-  <si>
     <t>lon</t>
   </si>
   <si>
     <t>lat</t>
   </si>
   <si>
-    <t>provincia</t>
-  </si>
-  <si>
     <t>data_arribada</t>
   </si>
   <si>
-    <t>comentaris</t>
-  </si>
-  <si>
     <t>inici_simptomes</t>
   </si>
   <si>
-    <t>edat</t>
-  </si>
-  <si>
     <t>estat</t>
   </si>
   <si>
-    <t>adreca</t>
-  </si>
-  <si>
     <t>pais_visitat</t>
+  </si>
+  <si>
+    <t>numero</t>
+  </si>
+  <si>
+    <t>centre_dia</t>
+  </si>
+  <si>
+    <t>any</t>
+  </si>
+  <si>
+    <t>prov</t>
+  </si>
+  <si>
+    <t>edatany</t>
+  </si>
+  <si>
+    <t>observacio</t>
   </si>
 </sst>
 </file>
@@ -400,7 +400,7 @@
   <dimension ref="A1:L10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="M9" sqref="M9"/>
+      <selection activeCell="L2" sqref="L2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -416,40 +416,40 @@
   <sheetData>
     <row r="1" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
+      <c r="D1" t="s">
+        <v>2</v>
+      </c>
+      <c r="E1" t="s">
         <v>3</v>
       </c>
-      <c r="C1" t="s">
-        <v>2</v>
-      </c>
-      <c r="D1" t="s">
+      <c r="F1" t="s">
         <v>5</v>
       </c>
-      <c r="E1" t="s">
+      <c r="G1" t="s">
+        <v>4</v>
+      </c>
+      <c r="H1" t="s">
         <v>7</v>
       </c>
-      <c r="F1" t="s">
+      <c r="I1" t="s">
+        <v>8</v>
+      </c>
+      <c r="J1" t="s">
+        <v>9</v>
+      </c>
+      <c r="K1" t="s">
+        <v>10</v>
+      </c>
+      <c r="L1" t="s">
         <v>11</v>
-      </c>
-      <c r="G1" t="s">
-        <v>9</v>
-      </c>
-      <c r="H1" t="s">
-        <v>1</v>
-      </c>
-      <c r="I1" t="s">
-        <v>10</v>
-      </c>
-      <c r="J1" t="s">
-        <v>4</v>
-      </c>
-      <c r="K1" t="s">
-        <v>8</v>
-      </c>
-      <c r="L1" t="s">
-        <v>6</v>
       </c>
     </row>
     <row r="3" spans="1:12" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Added field to epi metadata
</commit_message>
<xml_diff>
--- a/tigapublic/templates/epi/epi_template.xlsx
+++ b/tigapublic/templates/epi/epi_template.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="13">
   <si>
     <t>lon</t>
   </si>
@@ -50,6 +50,9 @@
   </si>
   <si>
     <t>observacio</t>
+  </si>
+  <si>
+    <t>data_notificacio</t>
   </si>
 </sst>
 </file>
@@ -397,24 +400,25 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:L10"/>
+  <dimension ref="A1:M10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L2" sqref="L2"/>
+      <selection activeCell="F1" sqref="F1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="4" max="4" width="13.140625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="15.7109375" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="15.7109375" customWidth="1"/>
-    <col min="7" max="7" width="13.140625" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="10.85546875" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="15.5703125" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="10.85546875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="15.140625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="15.7109375" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="15.7109375" customWidth="1"/>
+    <col min="8" max="8" width="13.140625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="10.85546875" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="15.5703125" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="10.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>6</v>
       </c>
@@ -428,39 +432,42 @@
         <v>2</v>
       </c>
       <c r="E1" t="s">
+        <v>12</v>
+      </c>
+      <c r="F1" t="s">
         <v>3</v>
       </c>
-      <c r="F1" t="s">
+      <c r="G1" t="s">
         <v>5</v>
       </c>
-      <c r="G1" t="s">
+      <c r="H1" t="s">
         <v>4</v>
       </c>
-      <c r="H1" t="s">
+      <c r="I1" t="s">
         <v>7</v>
       </c>
-      <c r="I1" t="s">
+      <c r="J1" t="s">
         <v>8</v>
       </c>
-      <c r="J1" t="s">
+      <c r="K1" t="s">
         <v>9</v>
       </c>
-      <c r="K1" t="s">
+      <c r="L1" t="s">
         <v>10</v>
       </c>
-      <c r="L1" t="s">
+      <c r="M1" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="E3" s="1"/>
+    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
       <c r="F3" s="1"/>
+      <c r="G3" s="1"/>
     </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="L6" s="1"/>
+    <row r="6" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="M6" s="1"/>
     </row>
-    <row r="10" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="I10" s="1"/>
+    <row r="10" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="J10" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>